<commit_message>
Updated all lookup table data files.
</commit_message>
<xml_diff>
--- a/IEDC_LookupTable_fill/aspects_data.xlsx
+++ b/IEDC_LookupTable_fill/aspects_data.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="99">
   <si>
     <t>id</t>
   </si>
@@ -40,9 +40,6 @@
     <t>reserve3</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Model time</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>Cohort</t>
-  </si>
-  <si>
     <t>age-cohorts</t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>cohort</t>
   </si>
   <si>
-    <t>Element</t>
-  </si>
-  <si>
     <t>chemical elements</t>
   </si>
   <si>
@@ -76,18 +67,12 @@
     <t>element</t>
   </si>
   <si>
-    <t>Unity</t>
-  </si>
-  <si>
     <t>trivial classification, 1 entry only</t>
   </si>
   <si>
     <t>1 (unity)</t>
   </si>
   <si>
-    <t>(Residence) region</t>
-  </si>
-  <si>
     <t>Region of process or stock</t>
   </si>
   <si>
@@ -97,9 +82,6 @@
     <t>region</t>
   </si>
   <si>
-    <t>OriginRegion</t>
-  </si>
-  <si>
     <t>Region of origin (flow)</t>
   </si>
   <si>
@@ -109,9 +91,6 @@
     <t>origin</t>
   </si>
   <si>
-    <t>DestinationRegion</t>
-  </si>
-  <si>
     <t>region of destination (flow)</t>
   </si>
   <si>
@@ -121,9 +100,6 @@
     <t>destination</t>
   </si>
   <si>
-    <t>(Residence) process</t>
-  </si>
-  <si>
     <t>Process where stock is located</t>
   </si>
   <si>
@@ -133,27 +109,18 @@
     <t>process</t>
   </si>
   <si>
-    <t>OriginProcess</t>
-  </si>
-  <si>
     <t>Process of origin of flow</t>
   </si>
   <si>
     <t>o</t>
   </si>
   <si>
-    <t>DestinationProcess</t>
-  </si>
-  <si>
     <t>Process of destination of flow</t>
   </si>
   <si>
     <t>d</t>
   </si>
   <si>
-    <t>Good,product</t>
-  </si>
-  <si>
     <t>Goods and products considered</t>
   </si>
   <si>
@@ -163,21 +130,9 @@
     <t>good</t>
   </si>
   <si>
-    <t>Engineering materials</t>
-  </si>
-  <si>
     <t>Engineering materials considered</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>alloy (and oll other engineering materials)</t>
-  </si>
-  <si>
-    <t>EoL_Goods</t>
-  </si>
-  <si>
     <t>End-of-life products, buildings, and infrastructure</t>
   </si>
   <si>
@@ -187,9 +142,6 @@
     <t>end-of-Life product</t>
   </si>
   <si>
-    <t>Waste_Scrap</t>
-  </si>
-  <si>
     <t>waste and scrap types considered</t>
   </si>
   <si>
@@ -199,12 +151,6 @@
     <t>waste/scrap</t>
   </si>
   <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>Energy consumed</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -220,9 +166,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>Extensions</t>
-  </si>
-  <si>
     <t>Costs, emissions factors, social impacts</t>
   </si>
   <si>
@@ -232,9 +175,6 @@
     <t>Xtension</t>
   </si>
   <si>
-    <t>Service</t>
-  </si>
-  <si>
     <t>Service categories: shelter, transport, etc.</t>
   </si>
   <si>
@@ -245,6 +185,132 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>substituting_material</t>
+  </si>
+  <si>
+    <t>age-cohort</t>
+  </si>
+  <si>
+    <t>unity</t>
+  </si>
+  <si>
+    <t>origin_region</t>
+  </si>
+  <si>
+    <t>destination_region</t>
+  </si>
+  <si>
+    <t>origin_process</t>
+  </si>
+  <si>
+    <t>destination_process</t>
+  </si>
+  <si>
+    <t>commodity</t>
+  </si>
+  <si>
+    <t>engineering_material</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>EoL_good</t>
+  </si>
+  <si>
+    <t>waste_scrap</t>
+  </si>
+  <si>
+    <t>energy_carrier</t>
+  </si>
+  <si>
+    <t>Energy carrier</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>extension</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>product_type</t>
+  </si>
+  <si>
+    <t>Types of products</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TYpe</t>
+  </si>
+  <si>
+    <t>input_material</t>
+  </si>
+  <si>
+    <t>Input of material to process</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>input_commodity</t>
+  </si>
+  <si>
+    <t>Input of commodity to process</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>output_material</t>
+  </si>
+  <si>
+    <t>Output of material to process</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>output_commodity</t>
+  </si>
+  <si>
+    <t>Output of commodity to process</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>technology</t>
+  </si>
+  <si>
+    <t>technology of product or commodity</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>material that is substituting another one</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>substituting …</t>
   </si>
 </sst>
 </file>
@@ -330,7 +396,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -632,19 +698,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="63.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -673,53 +739,53 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -727,30 +793,30 @@
         <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -759,335 +825,476 @@
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D6" s="8">
         <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4">
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4">
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D9" s="10">
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D10" s="10">
         <v>7</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D11" s="10">
         <v>7</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D12" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D13" s="4">
         <v>5</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D15" s="4">
         <v>5</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D16" s="4">
         <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D17" s="4">
         <v>9</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="D18" s="4">
         <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D19" s="11">
         <v>11</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="4"/>
     </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="11">
+        <v>6</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="11">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="11">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="11">
+        <v>6</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="11">
+        <v>5</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="4">
+        <v>6</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="11">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="5">
+        <v>6</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="11">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="5">
+        <v>5</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
revised table def and classification_structure.
</commit_message>
<xml_diff>
--- a/IEDC_LookupTable_fill/aspects_data.xlsx
+++ b/IEDC_LookupTable_fill/aspects_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
   <si>
     <t>id</t>
   </si>
@@ -356,6 +356,18 @@
   </si>
   <si>
     <t>material Category</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>City where process or stock is located, flows start or end</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Cit_y</t>
   </si>
 </sst>
 </file>
@@ -743,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O24:O25"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1418,6 +1430,26 @@
         <v>110</v>
       </c>
     </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="11">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="5">
+        <v>4</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>